<commit_message>
tidy up.  add hydrology.  add watershed code to priorities
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9293063-E8EB-45E4-A80B-5A77D7AA0389}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD9E423-3EB8-4BAC-A1C1-3216C961028C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
+    <workbookView xWindow="6360" yWindow="1485" windowWidth="21600" windowHeight="11385" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
   <sheets>
     <sheet name="priorities" sheetId="1" r:id="rId1"/>
     <sheet name="bt_critical" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$E$1:$E$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$F$1:$F$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
     <author>tc={62D18BF9-B4D1-4E85-A958-96B85D2D3486}</author>
   </authors>
   <commentList>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
   <si>
     <t>Good habitat. Particularly the lowest 200m.  Surveyed downstream for 700 m to confluence with Wichcika River.   Some deep pools for overwintering.  Occasional pockets of gravel suitable for spawning. Rock falls located approximately 75 mbelow the crossing would likely present barrier to all but adult adfluvial bull trout.  Abundant large woody debris througout.  Stable stream channel.</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t xml:space="preserve">Good habitat.  Surveyed downstream of PSCIS crossing 125186 for a distance of 350 m.  Young of year observed approximately 100 m downstream of crossing.  Abundant gravels throughout. Abandoned dry channels at bottom of suveyed area. Although we could not  immediately locate the watered channel during the survey it is likely not subsurface (at least for most of the year) based the quantity of flow upstream.  </t>
+  </si>
+  <si>
+    <t>200-948755-936902-729757-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000-000000</t>
+  </si>
+  <si>
+    <t>watershed_code</t>
   </si>
 </sst>
 </file>
@@ -745,7 +751,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="E10" dT="2020-04-18T20:31:59.51" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
+  <threadedComment ref="F10" dT="2020-04-18T20:31:59.51" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
     <text>flows into potential juv bt critical habitat</text>
   </threadedComment>
   <threadedComment ref="C21" dT="2020-03-02T16:45:41.92" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{62D18BF9-B4D1-4E85-A958-96B85D2D3486}">
@@ -756,20 +762,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="4" max="5" width="41.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -783,13 +789,16 @@
         <v>64</v>
       </c>
       <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
         <v>56</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -802,14 +811,14 @@
       <c r="D2" t="s">
         <v>60</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>58</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -822,14 +831,14 @@
       <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>58</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -842,14 +851,14 @@
       <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>58</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -862,14 +871,14 @@
       <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>58</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -882,14 +891,14 @@
       <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -902,14 +911,14 @@
       <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -922,14 +931,14 @@
       <c r="D8" t="s">
         <v>62</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>58</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -942,14 +951,14 @@
       <c r="D9" t="s">
         <v>62</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -962,14 +971,14 @@
       <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -982,14 +991,14 @@
       <c r="D11" t="s">
         <v>60</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>66</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1002,14 +1011,14 @@
       <c r="D12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>66</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1022,14 +1031,14 @@
       <c r="D13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>66</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1042,14 +1051,17 @@
       <c r="D14" t="s">
         <v>62</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1062,14 +1074,14 @@
       <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>59</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1082,14 +1094,14 @@
       <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>58</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1102,14 +1114,14 @@
       <c r="D17" t="s">
         <v>61</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>58</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1122,14 +1134,14 @@
       <c r="D18" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1142,14 +1154,14 @@
       <c r="D19" t="s">
         <v>63</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>59</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1162,11 +1174,11 @@
       <c r="D20" t="s">
         <v>62</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1179,11 +1191,11 @@
       <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1196,14 +1208,14 @@
       <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>66</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1216,14 +1228,14 @@
       <c r="D23" t="s">
         <v>63</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>66</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1236,11 +1248,11 @@
       <c r="D24" t="s">
         <v>62</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1253,11 +1265,11 @@
       <c r="D25" t="s">
         <v>62</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1270,14 +1282,14 @@
       <c r="D26" t="s">
         <v>62</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>59</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1290,14 +1302,14 @@
       <c r="D27" t="s">
         <v>62</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>59</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1310,11 +1322,11 @@
       <c r="D28" t="s">
         <v>62</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1327,14 +1339,15 @@
       <c r="D29" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1347,14 +1360,14 @@
       <c r="D30" t="s">
         <v>61</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1367,14 +1380,14 @@
       <c r="D31" t="s">
         <v>61</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1387,14 +1400,14 @@
       <c r="D32" t="s">
         <v>61</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>59</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1407,14 +1420,14 @@
       <c r="D33" t="s">
         <v>62</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>58</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1427,26 +1440,26 @@
       <c r="D34" t="s">
         <v>62</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>58</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C38">
         <f>SUM(C2:C35)</f>
         <v>14690</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
+  <autoFilter ref="F1:F38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
running with all high crossings sans photos.  Update photometa data with stuff i thouhgt i already saved...
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD9E423-3EB8-4BAC-A1C1-3216C961028C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863C44C4-CB97-472D-8595-0543D7B161A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1485" windowWidth="21600" windowHeight="11385" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
   <sheets>
     <sheet name="priorities" sheetId="1" r:id="rId1"/>
     <sheet name="bt_critical" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$F$1:$F$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$G$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
     <author>tc={62D18BF9-B4D1-4E85-A958-96B85D2D3486}</author>
   </authors>
   <commentList>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,19 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="102">
-  <si>
-    <t>Good habitat. Particularly the lowest 200m.  Surveyed downstream for 700 m to confluence with Wichcika River.   Some deep pools for overwintering.  Occasional pockets of gravel suitable for spawning. Rock falls located approximately 75 mbelow the crossing would likely present barrier to all but adult adfluvial bull trout.  Abundant large woody debris througout.  Stable stream channel.</t>
-  </si>
-  <si>
-    <t>Moderate value habitat.  Surveyed upstream for 650 m to impassable cascade. Some occasional pools. Frequent steps 30 - 50 cm due to large woody debris jams.  Mature spreuce forest. Cascade at top end of site not passable by any species or life stage. Good sized stream with som intermittent small paches of gravel suitable forspawning. Overall nice stream but unlikely overly important to adfluvial bull trout populations due to limited spawning habitat.  Too steep for rainbow access due to rock drop below the crossing.</t>
-  </si>
-  <si>
-    <t>Moderate to low value habitat. Surveyed upstream for 565 m.   Lack of large woody debris and no deep pools. At approximately 300m upstream of culvert stream spilts into three tributaries.  Western most tributary has the most flow.  Abundant gravels but very little to no overwintering habitat available if fish passage was restored at the crossing.</t>
-  </si>
-  <si>
-    <t>Moderate value habitat.  Surveyed downstream for 400 m.  Abundant gravels throughout.  No barriers in surveyed area.  No funcional large woody debris but abundant small woody debris and ndercut banks. Higher value habitat below the culvert than above.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="138">
   <si>
     <t xml:space="preserve">Good habitat.  Surveyed upstream for 520 m.  Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
   </si>
@@ -87,12 +75,6 @@
     <t>Surveyed upstream for approximately 350 m.  Beaver influenced wetland for first 50 m then small stream with deep polls and undercut banks, overhanging vegetation.  Large wetland upstream of beaver dam located at approx. 200m from crossing.  Fixing culvert provides access to plateau wetland areas and not a priority.</t>
   </si>
   <si>
-    <t>Survyed downstream for 120 m.  Very thick shrubs over stream with small channel meandering througout muddy substrate on floodplain of the Parsnip River.</t>
-  </si>
-  <si>
-    <t>Moderate habitat value. Surveyed upstream for 920 m.  Larger stream wth pockets of gravels, some shallow pools and some widely spaced large woody devris.  No bariers observed besides debris jams of 50 - 100cm.  These obstructions are non-permanent and likley navigateable at different flows and by large fish.</t>
-  </si>
-  <si>
     <t>Good habitat. Surveyed upstream for 650 m.  Large stream with many deep pools suitable for overwintering and rearing.  Multiple rock chutes up to 1 m high in surveyed area with 1.4 m falls at top end of ste.  Rainbow trout (120 mm) observd approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.  Falls only potentially passable for adfluvial bull trout and migration to this area seems unlikely given plateau topography and wetland character present upstream (based on google earth review).</t>
   </si>
   <si>
@@ -204,9 +186,6 @@
     <t xml:space="preserve">Good habitat.  Surveyed downstream for 520 m upstream of PCSIS crossing 57695 to beyond historic observation of bull trout.  Site is also labelled as PSCIS 125424.  Stable mature streambed with frequent pieces of functional large woody debris stepping channel to grade.  Extensive areas of gravels suitable for spawning.  Steps throughout up to 0.6 m in high due to large woody debris.  </t>
   </si>
   <si>
-    <t>Good habitat.  Surveyed to 700 m upstream where beaver dammed area begins. Abundant undercut banks, overhanging vegetation, large woody debris and gravels. Gradinets decreasing at top end of the site due to historic beaver dam.  Railway culvert (modelled crossing 16603287) is located approximately 200 m upstream and is barrier (very long, unembedded and 3%).</t>
-  </si>
-  <si>
     <t>Good habitat.  Surveyed 230 m downstream to confluence of Parsnip River.  Wanders through floodplain of Parsnip River.  No barriers.</t>
   </si>
   <si>
@@ -228,9 +207,6 @@
     <t xml:space="preserve">Good habitat.  Suveyed downstream of crossing for 380 m.  Abundant gravels throughout with undercut banks, overhanging vegetation.  Mature forest with open shrubby riparian.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Moderate habitat.  Surveyed upstream for 285 m.  Small streawm with low flow indicated by moss mid-channel.  Very few polls but sections of gravel present.  Fish bearing according to FISS records. </t>
-  </si>
-  <si>
     <t>Moderate value habitat.  Surveyed downsteam of crossing PSCIS crossing 125098 for 175 m.  Small stream with low flows.  Fish records indicate fish observed upstream.</t>
   </si>
   <si>
@@ -354,15 +330,6 @@
     <t>Good habitat.  Surveyed for 600m to new bridge (modelled crossing 16603641).  Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high.  No persistent barriers.  Rainbow trout known upstream (FIDQ 2020). Good candidate for rehabilitation.</t>
   </si>
   <si>
-    <t xml:space="preserve">Good habitat.  Surveyed upstream for 680 m.  Culvert is under the Chuchinka-Colbourne FSR but railway located 10 m upstream also has barrier crossing (PSCIS 125345).  Abundant gravels throughout with deep pools suitable for overwintering.  No barriers.  Small beaver dam located 180 m upstream of crossing.  </t>
-  </si>
-  <si>
-    <t>Good habitat. Surveyed upstream for 700 m from crossing.  Larger stream with good flow and habiat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris.  Good candidate for rehabilitation.</t>
-  </si>
-  <si>
-    <t>Good habitat.  Surveyed upstream of PSCIS crossing 125186 for a distance of 515 m.  Good flow and abundant cover.  Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. Good candidate.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Good habitat.  Surveyed downstream of PSCIS crossing 125186 for a distance of 350 m.  Young of year observed approximately 100 m downstream of crossing.  Abundant gravels throughout. Abandoned dry channels at bottom of suveyed area. Although we could not  immediately locate the watered channel during the survey it is likely not subsurface (at least for most of the year) based the quantity of flow upstream.  </t>
   </si>
   <si>
@@ -370,6 +337,147 @@
   </si>
   <si>
     <t>watershed_code</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good habitat.  Surveyed upstream for 680 m.  Culvert is under the Chuchinka-Colbourne FSR but CN railway located 10 m upstream also has barrier crossing (PSCIS 125345).  Abundant gravels throughout with deep pools suitable for overwintering.  No barriers.  Small beaver dam located 180 m upstream of crossing.  </t>
+  </si>
+  <si>
+    <t>Good habitat. Surveyed upstream for 700 m from crossing.  Larger stream with good flow and high habitat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris.  Good candidate for rehabilitation.</t>
+  </si>
+  <si>
+    <t>Good habitat.  Surveyed upstream of crossing for a distance of 515 m.  Good flow and abundant cover.  Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. Good candidate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderate habitat.  Surveyed upstream for 285 m.  Small stream with low flow indicated by moss mid-channel.  Very few polls but sections of gravel present.  Fish bearing according to FISS records. </t>
+  </si>
+  <si>
+    <t>hab_value</t>
+  </si>
+  <si>
+    <t>Surveyed upstream for 565 m.   Lack of large woody debris and no deep pools. At approximately 300m upstream of culvert stream spilts into three tributaries.  Abundant gravels but very little to no overwintering habitat available if fish passage was restored at the crossing.</t>
+  </si>
+  <si>
+    <t>comments_for_submission</t>
+  </si>
+  <si>
+    <t>Surveyed downstream for 700 m to confluence with Wichcika River. Particularly good habitat in the lowest 200m.   Some deep pools for overwintering.  Occasional pockets of gravel suitable for spawning. Rock falls located approximately 75 m below the crossing would likely present barrier to all but adult adfluvial bull trout.  Abundant large woody debris througout.  Stable stream channel.</t>
+  </si>
+  <si>
+    <t>Some deep pools for overwintering and occasional pockets of gravel suitable for spawning. Rock falls 75 m below the crossing would likely present barrier to all but adult adfluvial bull trout.  Abundant large woody debris througout.  Stable stream channel.</t>
+  </si>
+  <si>
+    <t>Surveyed upstream for 650 m to impassable cascade. Some occasional pools. Frequent steps 30 - 50 cm due to large woody debris jams.  Mature spruce forest. Cascade at top end of site not passable by any species or life stage. Good sized stream with some intermittent small paches of gravel suitable for spawning. Overall nice stream but unlikely overly important to adfluvial bull trout populations due to limited spawning habitat.  Too steep for rainbow access due to rock drop below the crossing.</t>
+  </si>
+  <si>
+    <t>Cascade at top end of site (650 m upstream) not passable by any species or life stage. Some intermittent small paches of gravel suitable for spawning. Very limited spawning habitat.</t>
+  </si>
+  <si>
+    <t>At approximately 300m upstream of culvert stream spilts into three tributaries.  Abundant gravels but very little to no overwintering habitat.  Lack of large woody debris and no deep pools.</t>
+  </si>
+  <si>
+    <t>Surveyed downstream for 400 m.  Abundant gravels throughout.  No barriers in surveyed area.  No functional large woody debris but abundant small woody debris and undercut banks. Higher value habitat below the culvert than above.</t>
+  </si>
+  <si>
+    <t>Abundant gravels throughout.   No functional large woody debris but abundant small woody debris and undercut banks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
+  </si>
+  <si>
+    <t>Abundant large woody debris and gravels suitable for spawning.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Beaver influenced wetland for first 50 m then small stream with deep polls and undercut banks, overhanging vegetation.  Large wetland approximatly 200m upstream of crossing.</t>
+  </si>
+  <si>
+    <t>Surveyed downstream for 120 m.  Very thick shrubs over stream with small channel meandering througout muddy substrate on floodplain of the Parsnip River.</t>
+  </si>
+  <si>
+    <t>Very thick shrubs over stream with small channel meandering througout muddy substrate on floodplain of the Parsnip River.</t>
+  </si>
+  <si>
+    <t>Stable mature streambed with frequent pieces of functional large woody debris stepping channel to grade.  Extensive areas of gravels suitable for spawning.  Steps throughout up to 0.6 m in high due to large woody debris.</t>
+  </si>
+  <si>
+    <t>Moderate habitat value. Surveyed upstream for 920 m.  Larger stream wth pockets of gravels, some shallow pools and some widely spaced large woody debris.  No bariers observed besides debris jams ranging from 50 - 100 cm in height.  These obstructions are non-permanent and likley navigateable at different flows and by large fish.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pockets of gravels, some shallow pools and some widely spaced large woody debris.  No bariers observed besides debris jams ranging from 50 - 100 cm in height. </t>
+  </si>
+  <si>
+    <t>Multiple rock chutes up to 1 m high in surveyed area with 1.4 m falls at top end of ste.  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observd approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Uncomplex habitat with very occasional shallow pools.  Large woody debris infrequent.  Some patches of gravels present suitable for spawning.</t>
+  </si>
+  <si>
+    <t>Minnowtrapping conducted upstream and downstream of crossing with Rainbow Trout and Sculpin captured downstream. Undercut banks, large woody debris and overhanging vegetation througout.  Pools shallow. Beaver dams start 330m upstream of crossing.</t>
+  </si>
+  <si>
+    <t>Beaver influencced wetland/stream complex below crossing.  Deep glide habitat throughout (90 cm deep at time of survey).</t>
+  </si>
+  <si>
+    <t>Beaver influenced extensive wetland area located upstream for as far as visible from 50 m upstream of culvert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 m high cascde (10 m long at 50% gradient) is located approximately 5 m below the culvert.  Below this is a rock chute for 12 m (30%).</t>
+  </si>
+  <si>
+    <t>Abundant gravels thoroughout.  Multiple side channels. Some deeper pools.   Railway culvert modelled as 16603641 is located downstream and is embeded and passable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. New bridge upstream.</t>
+  </si>
+  <si>
+    <t>Good habitat.  Surveyed to 700 m upstream where beaver dammed area begins. Abundant undercut banks, overhanging vegetation, large woody debris and gravels. Gradients decreasing at top end of the site due to historic beaver dam.  Railway culvert (modelled crossing 16603287) is located approximately 200 m upstream and is barrier (very long, unembedded and 3%).</t>
+  </si>
+  <si>
+    <t>Abundant undercut banks, overhanging vegetation, large woody debris and gravels.  Historic beaver dam 700 m upstream.  Railway culvert (modelled crossing 16603287) is  200 m upstream and is barrier (very long, unembedded and 3%).</t>
+  </si>
+  <si>
+    <t>Wanders through floodplain of Parsnip River.  No barriers.</t>
+  </si>
+  <si>
+    <t>Abundant gravels throughout.  Some deep pools, undercut banks and large woody debris present.</t>
+  </si>
+  <si>
+    <t>Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream.  20 cm long bull trout observed approximately 340 m upstream of the culvert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Railway crossing culvert 16603267 is technically a barrier and located downstream of the crossing at the downstream end of the site. </t>
+  </si>
+  <si>
+    <t>Stable channel with large woody debris throughout.  Overhanging vegetation and undercut banks present for cover. Historic beaver impounded area at top of site.</t>
+  </si>
+  <si>
+    <t>Culvert is under the Chuchinka-Colbourne FSR but CN railway located 10 m upstream also has barrier crossing. Abundant gravels throughout with deep pools suitable for overwintering.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonids and cyprinids observed downstream throughout. Beaver activity with breached dam present.  Hunting/fishing camp located near confluence of Parsnip River. </t>
+  </si>
+  <si>
+    <t>Culvert is very long, steep and continous under the CN railway and Anzac FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larger stream with good flow and high habitat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris. </t>
+  </si>
+  <si>
+    <t>Abundant gravels throughout with undercut banks, overhanging vegetation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. </t>
+  </si>
+  <si>
+    <t>Young of year observed approximately 100 m downstream of crossing.  Abundant gravels throughout.</t>
+  </si>
+  <si>
+    <t>Small stream with low flow indicated by moss mid-channel.  Very few polls but sections of gravel present.</t>
+  </si>
+  <si>
+    <t>Small stream with low flows.</t>
   </si>
 </sst>
 </file>
@@ -751,7 +859,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="F10" dT="2020-04-18T20:31:59.51" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
+  <threadedComment ref="G10" dT="2020-04-18T20:31:59.51" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
     <text>flows into potential juv bt critical habitat</text>
   </threadedComment>
   <threadedComment ref="C21" dT="2020-03-02T16:45:41.92" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{62D18BF9-B4D1-4E85-A958-96B85D2D3486}">
@@ -762,704 +870,924 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="41.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="8" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>700</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>650</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="G3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>565</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>400</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>520</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>360</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>350</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H8" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>520</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C11">
         <v>920</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <v>650</v>
       </c>
       <c r="D12" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C13">
         <v>260</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="G13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>350</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>325</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H15" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>350</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <v>600</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H19" t="s">
+        <v>121</v>
+      </c>
+      <c r="I19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20">
         <v>755</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H20" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>190</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H21" t="s">
+        <v>124</v>
+      </c>
+      <c r="I21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C22">
         <v>310</v>
       </c>
       <c r="D22" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F22" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H22" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C23">
         <v>425</v>
       </c>
       <c r="D23" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
+        <v>126</v>
+      </c>
+      <c r="I23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C24">
         <v>800</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H24" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25">
         <v>240</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
       </c>
       <c r="G25" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>128</v>
+      </c>
+      <c r="I25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C26">
         <v>680</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H26" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C27">
         <v>220</v>
       </c>
       <c r="D27" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H27" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C28">
         <v>550</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="F28" t="s">
+        <v>91</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="H28" t="s">
+        <v>131</v>
+      </c>
+      <c r="I28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C29" s="2">
         <v>530</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C30">
         <v>600</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G30" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H30" t="s">
+        <v>133</v>
+      </c>
+      <c r="I30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C31">
         <v>400</v>
       </c>
       <c r="D31" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="I31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C32">
         <v>525</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G32" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="H32" t="s">
+        <v>135</v>
+      </c>
+      <c r="I32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C33">
         <v>295</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="G33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H33" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C34">
         <v>215</v>
       </c>
       <c r="D34" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F34" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="G34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="H34" t="s">
+        <v>137</v>
+      </c>
+      <c r="I34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C38">
         <f>SUM(C2:C35)</f>
         <v>14690</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
+  <autoFilter ref="G1:G38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1478,31 +1806,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
         <v>79</v>
       </c>
-      <c r="B1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" t="s">
-        <v>87</v>
-      </c>
       <c r="H1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="I1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1510,19 +1838,19 @@
         <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -1539,19 +1867,19 @@
         <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G3">
         <v>10</v>
@@ -1568,19 +1896,19 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G4">
         <v>10</v>
@@ -1597,19 +1925,19 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G5">
         <v>10</v>

</xml_diff>

<commit_message>
Add CV1 photos.  Upgdate CV1 to high priority.
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863C44C4-CB97-472D-8595-0543D7B161A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065FE85-E2BC-4C97-BCA4-8D535C59B5D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
@@ -360,9 +360,6 @@
     <t>Surveyed upstream for 565 m.   Lack of large woody debris and no deep pools. At approximately 300m upstream of culvert stream spilts into three tributaries.  Abundant gravels but very little to no overwintering habitat available if fish passage was restored at the crossing.</t>
   </si>
   <si>
-    <t>comments_for_submission</t>
-  </si>
-  <si>
     <t>Surveyed downstream for 700 m to confluence with Wichcika River. Particularly good habitat in the lowest 200m.   Some deep pools for overwintering.  Occasional pockets of gravel suitable for spawning. Rock falls located approximately 75 m below the crossing would likely present barrier to all but adult adfluvial bull trout.  Abundant large woody debris througout.  Stable stream channel.</t>
   </si>
   <si>
@@ -414,9 +411,6 @@
     <t xml:space="preserve"> Uncomplex habitat with very occasional shallow pools.  Large woody debris infrequent.  Some patches of gravels present suitable for spawning.</t>
   </si>
   <si>
-    <t>Minnowtrapping conducted upstream and downstream of crossing with Rainbow Trout and Sculpin captured downstream. Undercut banks, large woody debris and overhanging vegetation througout.  Pools shallow. Beaver dams start 330m upstream of crossing.</t>
-  </si>
-  <si>
     <t>Beaver influencced wetland/stream complex below crossing.  Deep glide habitat throughout (90 cm deep at time of survey).</t>
   </si>
   <si>
@@ -429,36 +423,18 @@
     <t>Abundant gravels thoroughout.  Multiple side channels. Some deeper pools.   Railway culvert modelled as 16603641 is located downstream and is embeded and passable.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. New bridge upstream.</t>
-  </si>
-  <si>
     <t>Good habitat.  Surveyed to 700 m upstream where beaver dammed area begins. Abundant undercut banks, overhanging vegetation, large woody debris and gravels. Gradients decreasing at top end of the site due to historic beaver dam.  Railway culvert (modelled crossing 16603287) is located approximately 200 m upstream and is barrier (very long, unembedded and 3%).</t>
   </si>
   <si>
-    <t>Abundant undercut banks, overhanging vegetation, large woody debris and gravels.  Historic beaver dam 700 m upstream.  Railway culvert (modelled crossing 16603287) is  200 m upstream and is barrier (very long, unembedded and 3%).</t>
-  </si>
-  <si>
     <t>Wanders through floodplain of Parsnip River.  No barriers.</t>
   </si>
   <si>
     <t>Abundant gravels throughout.  Some deep pools, undercut banks and large woody debris present.</t>
   </si>
   <si>
-    <t>Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream.  20 cm long bull trout observed approximately 340 m upstream of the culvert</t>
-  </si>
-  <si>
     <t xml:space="preserve">Railway crossing culvert 16603267 is technically a barrier and located downstream of the crossing at the downstream end of the site. </t>
   </si>
   <si>
-    <t>Stable channel with large woody debris throughout.  Overhanging vegetation and undercut banks present for cover. Historic beaver impounded area at top of site.</t>
-  </si>
-  <si>
-    <t>Culvert is under the Chuchinka-Colbourne FSR but CN railway located 10 m upstream also has barrier crossing. Abundant gravels throughout with deep pools suitable for overwintering.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salmonids and cyprinids observed downstream throughout. Beaver activity with breached dam present.  Hunting/fishing camp located near confluence of Parsnip River. </t>
-  </si>
-  <si>
     <t>Culvert is very long, steep and continous under the CN railway and Anzac FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
   </si>
   <si>
@@ -478,6 +454,30 @@
   </si>
   <si>
     <t>Small stream with low flows.</t>
+  </si>
+  <si>
+    <t>comments_for_submission_with_fish_permit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undercut banks, large woody debris and overhanging vegetation througout.  Pools shallow. Beaver dams start 330m upstream of crossing. Minnowtrapping conducted upstream and downstream of crossing with Rainbow Trout and Sculpin captured downstream. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. Passble railway culvert located downstream (16603641). New bridge upstream.</t>
+  </si>
+  <si>
+    <t>CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salmonids and cyprinids observed downstream throughout. Beaver activity with breached dam present.  Hunting/fishing camp located just downstream of crossing near confluence of Parsnip River. </t>
+  </si>
+  <si>
+    <t>Culvert is under Chuchinka-Colbourne FSR but CN railway crossing (PSCIS 57687) is  located 10 m upstream and also has barrier crossing. Abundant gravels throughout with deep pools suitable for overwintering.</t>
+  </si>
+  <si>
+    <t>Stable channel with large woody debris throughout.  Railway crossing culvert (modelled ID 16603267) is located 60 m downstream of the crossing and is a barrier. Overhanging vegetation and undercut banks present for cover. Historic beaver impounded area at top of site.</t>
+  </si>
+  <si>
+    <t>Abundant undercut banks, overhanging vegetation, large woody debris and gravels.  Historic beaver dam 700 m upstream.  Railway culvert (modelled crossing 16603287) is  200 m upstream and is barrier (90 m long, unembedded and 3%).</t>
   </si>
 </sst>
 </file>
@@ -870,10 +870,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,10 +911,10 @@
         <v>57</v>
       </c>
       <c r="I1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -933,13 +934,13 @@
         <v>50</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -959,13 +960,13 @@
         <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -985,13 +986,13 @@
         <v>50</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1011,10 +1012,10 @@
         <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1037,7 +1038,7 @@
         <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -1063,13 +1064,13 @@
         <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1089,13 +1090,13 @@
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1115,13 +1116,13 @@
         <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1141,13 +1142,13 @@
         <v>58</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1167,13 +1168,13 @@
         <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1193,13 +1194,13 @@
         <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I13" t="s">
         <v>4</v>
@@ -1248,7 +1249,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="I14" t="s">
         <v>84</v>
@@ -1274,13 +1275,13 @@
         <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1300,13 +1301,13 @@
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1326,7 +1327,7 @@
         <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
@@ -1352,7 +1353,7 @@
         <v>51</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I18" t="s">
         <v>86</v>
@@ -1378,7 +1379,7 @@
         <v>51</v>
       </c>
       <c r="H19" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="I19" t="s">
         <v>87</v>
@@ -1404,10 +1405,10 @@
         <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="I20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1430,7 +1431,7 @@
         <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I21" t="s">
         <v>40</v>
@@ -1453,10 +1454,10 @@
         <v>51</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I22" t="s">
         <v>41</v>
@@ -1479,10 +1480,10 @@
         <v>51</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="I23" t="s">
         <v>42</v>
@@ -1508,7 +1509,7 @@
         <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I24" t="s">
         <v>43</v>
@@ -1534,7 +1535,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="I25" t="s">
         <v>44</v>
@@ -1560,7 +1561,7 @@
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="I26" t="s">
         <v>92</v>
@@ -1586,13 +1587,13 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="I27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1612,7 +1613,7 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I28" t="s">
         <v>45</v>
@@ -1639,7 +1640,7 @@
         <v>51</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>93</v>
@@ -1665,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I30" t="s">
         <v>46</v>
@@ -1691,7 +1692,7 @@
         <v>51</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="I31" t="s">
         <v>94</v>
@@ -1717,13 +1718,13 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1743,13 +1744,13 @@
         <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="I33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1769,25 +1770,33 @@
         <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="I34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>190</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="C38">
         <f>SUM(C2:C35)</f>
         <v>14690</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
+  <autoFilter ref="G1:G38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="High"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
add sensitive watershed info and georeference photos for CV1
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9065FE85-E2BC-4C97-BCA4-8D535C59B5D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD02E08-3CF4-40CE-8D42-00396209FDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
@@ -381,9 +381,6 @@
     <t>Abundant gravels throughout.   No functional large woody debris but abundant small woody debris and undercut banks.</t>
   </si>
   <si>
-    <t xml:space="preserve">Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
-  </si>
-  <si>
     <t>Abundant large woody debris and gravels suitable for spawning.</t>
   </si>
   <si>
@@ -438,15 +435,9 @@
     <t>Culvert is very long, steep and continous under the CN railway and Anzac FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
   </si>
   <si>
-    <t xml:space="preserve">Larger stream with good flow and high habitat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris. </t>
-  </si>
-  <si>
     <t>Abundant gravels throughout with undercut banks, overhanging vegetation.</t>
   </si>
   <si>
-    <t xml:space="preserve">Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. </t>
-  </si>
-  <si>
     <t>Young of year observed approximately 100 m downstream of crossing.  Abundant gravels throughout.</t>
   </si>
   <si>
@@ -462,12 +453,6 @@
     <t xml:space="preserve">Undercut banks, large woody debris and overhanging vegetation througout.  Pools shallow. Beaver dams start 330m upstream of crossing. Minnowtrapping conducted upstream and downstream of crossing with Rainbow Trout and Sculpin captured downstream. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. Passble railway culvert located downstream (16603641). New bridge upstream.</t>
-  </si>
-  <si>
-    <t>CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Salmonids and cyprinids observed downstream throughout. Beaver activity with breached dam present.  Hunting/fishing camp located just downstream of crossing near confluence of Parsnip River. </t>
   </si>
   <si>
@@ -478,6 +463,21 @@
   </si>
   <si>
     <t>Abundant undercut banks, overhanging vegetation, large woody debris and gravels.  Historic beaver dam 700 m upstream.  Railway culvert (modelled crossing 16603287) is  200 m upstream and is barrier (90 m long, unembedded and 3%).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Larger stream with good flow and high habitat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. Passble railway culvert located downstream (16603641). New bridge upstream.</t>
+  </si>
+  <si>
+    <t>Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +911,7 @@
         <v>57</v>
       </c>
       <c r="I1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -1064,7 +1064,7 @@
         <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I7" t="s">
         <v>1</v>
@@ -1090,7 +1090,7 @@
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
@@ -1116,10 +1116,10 @@
         <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>58</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I10" t="s">
         <v>39</v>
@@ -1168,10 +1168,10 @@
         <v>58</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -1194,7 +1194,7 @@
         <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I12" t="s">
         <v>3</v>
@@ -1220,7 +1220,7 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I13" t="s">
         <v>4</v>
@@ -1249,7 +1249,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I14" t="s">
         <v>84</v>
@@ -1275,7 +1275,7 @@
         <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I15" t="s">
         <v>85</v>
@@ -1301,7 +1301,7 @@
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I16" t="s">
         <v>5</v>
@@ -1327,7 +1327,7 @@
         <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
@@ -1353,7 +1353,7 @@
         <v>51</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I18" t="s">
         <v>86</v>
@@ -1379,7 +1379,7 @@
         <v>51</v>
       </c>
       <c r="H19" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="I19" t="s">
         <v>87</v>
@@ -1405,10 +1405,10 @@
         <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I21" t="s">
         <v>40</v>
@@ -1457,7 +1457,7 @@
         <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I22" t="s">
         <v>41</v>
@@ -1483,7 +1483,7 @@
         <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="I23" t="s">
         <v>42</v>
@@ -1509,7 +1509,7 @@
         <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I24" t="s">
         <v>43</v>
@@ -1535,7 +1535,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I25" t="s">
         <v>44</v>
@@ -1561,7 +1561,7 @@
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I26" t="s">
         <v>92</v>
@@ -1587,7 +1587,7 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="I27" t="s">
         <v>83</v>
@@ -1613,7 +1613,7 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I28" t="s">
         <v>45</v>
@@ -1640,7 +1640,7 @@
         <v>51</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>93</v>
@@ -1666,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I30" t="s">
         <v>46</v>
@@ -1692,7 +1692,7 @@
         <v>51</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="I31" t="s">
         <v>94</v>
@@ -1718,7 +1718,7 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I32" t="s">
         <v>88</v>
@@ -1744,7 +1744,7 @@
         <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I33" t="s">
         <v>95</v>
@@ -1770,7 +1770,7 @@
         <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I34" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
update zipped kmls and road names in tables.  Add 125153
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD02E08-3CF4-40CE-8D42-00396209FDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156520A0-18E9-4E73-A1FE-7BCD9CCD0980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
@@ -477,7 +477,7 @@
     <t xml:space="preserve"> Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. Passble railway culvert located downstream (16603641). New bridge upstream.</t>
   </si>
   <si>
-    <t>Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
+    <t>Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream on FSRs.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
   </si>
 </sst>
 </file>
@@ -874,7 +874,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
tidy crossing details on map.  change medium priority to yellow.  Clean out some photos
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156520A0-18E9-4E73-A1FE-7BCD9CCD0980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E99DF-4BF5-4BE2-8E7E-F63CA8DF72E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
+    <workbookView xWindow="-21675" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
   <sheets>
     <sheet name="priorities" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t xml:space="preserve">Pockets of gravels, some shallow pools and some widely spaced large woody debris.  No bariers observed besides debris jams ranging from 50 - 100 cm in height. </t>
   </si>
   <si>
-    <t>Multiple rock chutes up to 1 m high in surveyed area with 1.4 m falls at top end of ste.  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observd approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Uncomplex habitat with very occasional shallow pools.  Large woody debris infrequent.  Some patches of gravels present suitable for spawning.</t>
   </si>
   <si>
@@ -432,9 +429,6 @@
     <t xml:space="preserve">Railway crossing culvert 16603267 is technically a barrier and located downstream of the crossing at the downstream end of the site. </t>
   </si>
   <si>
-    <t>Culvert is very long, steep and continous under the CN railway and Anzac FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
-  </si>
-  <si>
     <t>Abundant gravels throughout with undercut banks, overhanging vegetation.</t>
   </si>
   <si>
@@ -478,6 +472,12 @@
   </si>
   <si>
     <t>Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream on FSRs.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
+  </si>
+  <si>
+    <t>Culvert is very long, steep and continous under the CN railway and Chuchinka-Colbourne FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
+  </si>
+  <si>
+    <t>Multiple rock chutes up to 1 m high in surveyed area with 1.4 m falls at top end of ste.  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observed approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
   </si>
 </sst>
 </file>
@@ -870,11 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,10 +910,10 @@
         <v>57</v>
       </c>
       <c r="I1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -940,7 +939,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -966,7 +965,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -992,7 +991,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1038,7 +1037,7 @@
         <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -1070,7 +1069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1096,7 +1095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1122,7 +1121,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1148,7 +1147,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1174,7 +1173,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1194,13 +1193,13 @@
         <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>112</v>
+        <v>137</v>
       </c>
       <c r="I12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1220,7 +1219,7 @@
         <v>58</v>
       </c>
       <c r="H13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I13" t="s">
         <v>4</v>
@@ -1249,7 +1248,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I14" t="s">
         <v>84</v>
@@ -1275,13 +1274,13 @@
         <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I15" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1301,13 +1300,13 @@
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1327,7 +1326,7 @@
         <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
@@ -1353,7 +1352,7 @@
         <v>51</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I18" t="s">
         <v>86</v>
@@ -1379,7 +1378,7 @@
         <v>51</v>
       </c>
       <c r="H19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I19" t="s">
         <v>87</v>
@@ -1405,10 +1404,10 @@
         <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1431,7 +1430,7 @@
         <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I21" t="s">
         <v>40</v>
@@ -1457,7 +1456,7 @@
         <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I22" t="s">
         <v>41</v>
@@ -1483,7 +1482,7 @@
         <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I23" t="s">
         <v>42</v>
@@ -1509,7 +1508,7 @@
         <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I24" t="s">
         <v>43</v>
@@ -1535,7 +1534,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I25" t="s">
         <v>44</v>
@@ -1561,7 +1560,7 @@
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I26" t="s">
         <v>92</v>
@@ -1587,13 +1586,13 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I27" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="I28" t="s">
         <v>45</v>
@@ -1640,7 +1639,7 @@
         <v>51</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>93</v>
@@ -1666,7 +1665,7 @@
         <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I30" t="s">
         <v>46</v>
@@ -1692,7 +1691,7 @@
         <v>51</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I31" t="s">
         <v>94</v>
@@ -1718,13 +1717,13 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1744,13 +1743,13 @@
         <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I33" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1770,33 +1769,25 @@
         <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C35">
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C38">
         <f>SUM(C2:C35)</f>
         <v>14690</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="High"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="G1:G38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
update CV1 HGI and fish species. Correct text in priorities doc related to FSW
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{764E99DF-4BF5-4BE2-8E7E-F63CA8DF72E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1BC70B-F16C-4E63-9671-DA3EE23DF52B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21675" yWindow="690" windowWidth="21600" windowHeight="11385" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
   <sheets>
     <sheet name="priorities" sheetId="1" r:id="rId1"/>
@@ -459,25 +459,25 @@
     <t>Abundant undercut banks, overhanging vegetation, large woody debris and gravels.  Historic beaver dam 700 m upstream.  Railway culvert (modelled crossing 16603287) is  200 m upstream and is barrier (90 m long, unembedded and 3%).</t>
   </si>
   <si>
-    <t xml:space="preserve">Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Larger stream with good flow and high habitat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. Passble railway culvert located downstream (16603641). New bridge upstream.</t>
-  </si>
-  <si>
-    <t>Classified as fisheries sensitive watershed ander FRPA for Bull Trout and Arctic Grayling (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream on FSRs.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream.</t>
-  </si>
-  <si>
     <t>Culvert is very long, steep and continous under the CN railway and Chuchinka-Colbourne FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
   </si>
   <si>
     <t>Multiple rock chutes up to 1 m high in surveyed area with 1.4 m falls at top end of ste.  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observed approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling  (Beaudry 2014, FSW-TAG f-7-022). Some deep pools and boulders, udercut banks,  large wody debris and gravels throughout.   Some debris steps from 30 - 70 cms high. Passble railway culvert located downstream (16603641). New bridge upstream.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling  (Beaudry 2013, FSW-TAG f-7-020). Larger stream with good flow and high habitat complexity.  Frequent pockets of gravel suitable for spawing at pool tailouts and behind large woody debris. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Large woody debris and pools throughout.  Frequent pockets of gravel suitable for spawning. </t>
+  </si>
+  <si>
+    <t>Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling  (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream on FSRs.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream. 200mm Bull Trout (suspected) observed upstream near redd.</t>
   </si>
 </sst>
 </file>
@@ -872,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,7 +881,8 @@
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="41.85546875" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="8" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="88.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1037,7 +1038,7 @@
         <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -1193,7 +1194,7 @@
         <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="I12" t="s">
         <v>3</v>
@@ -1482,7 +1483,7 @@
         <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="I23" t="s">
         <v>42</v>
@@ -1612,7 +1613,7 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="I28" t="s">
         <v>45</v>
@@ -1639,7 +1640,7 @@
         <v>51</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>93</v>
@@ -1691,7 +1692,7 @@
         <v>51</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="I31" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
add 57681 photos.  updated priority and pscis_phas2 sheet with missing data
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1BC70B-F16C-4E63-9671-DA3EE23DF52B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD52AF2-4E16-4F3F-BAF6-5ECFBB24F8B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
@@ -405,12 +405,6 @@
     <t xml:space="preserve"> Uncomplex habitat with very occasional shallow pools.  Large woody debris infrequent.  Some patches of gravels present suitable for spawning.</t>
   </si>
   <si>
-    <t>Beaver influencced wetland/stream complex below crossing.  Deep glide habitat throughout (90 cm deep at time of survey).</t>
-  </si>
-  <si>
-    <t>Beaver influenced extensive wetland area located upstream for as far as visible from 50 m upstream of culvert.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 5 m high cascde (10 m long at 50% gradient) is located approximately 5 m below the culvert.  Below this is a rock chute for 12 m (30%).</t>
   </si>
   <si>
@@ -478,6 +472,12 @@
   </si>
   <si>
     <t>Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling  (Beaudry 2014, FSW-TAG f-7-022). CN Rail crossing.  Abundant gravels, large woody debris, undercut banks, overhanging vegetation and small woody debris. Recently installed bridges downsteam and upstream on FSRs.  20 cm long bull trout (suspected) observed approximately 340 m upstream of the culvert.  Minnowtrapping conducted upstream and downstream with Rainbow Trout captured downstream. 200mm Bull Trout (suspected) observed upstream near redd.</t>
+  </si>
+  <si>
+    <t>Beaver influenced extensive wetland area located upstream for as far as visible from 50 m upstream of culvert.   5 m high cascde (10 m long at 50% gradient) is located approximately 5 m below the culvert.  Below this is a rock chute for 12 m (30%). Culvert is potentially accessible only to adult adfluvial bull trout however it is unlikely that they would utilize this stream due to the wetland type habitat present upstream of the culvert.</t>
+  </si>
+  <si>
+    <t>Beaver influenced wetland/stream complex below crossing.  Deep glide habitat throughout (90 cm deep at time of survey).</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +911,7 @@
         <v>57</v>
       </c>
       <c r="I1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I6" t="s">
         <v>0</v>
@@ -1194,7 +1194,7 @@
         <v>58</v>
       </c>
       <c r="H12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I12" t="s">
         <v>3</v>
@@ -1249,7 +1249,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I14" t="s">
         <v>84</v>
@@ -1275,7 +1275,7 @@
         <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="I15" t="s">
         <v>85</v>
@@ -1301,7 +1301,7 @@
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="I16" t="s">
         <v>5</v>
@@ -1327,7 +1327,7 @@
         <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I17" t="s">
         <v>6</v>
@@ -1353,7 +1353,7 @@
         <v>51</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I18" t="s">
         <v>86</v>
@@ -1379,7 +1379,7 @@
         <v>51</v>
       </c>
       <c r="H19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I19" t="s">
         <v>87</v>
@@ -1405,10 +1405,10 @@
         <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1431,7 +1431,7 @@
         <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I21" t="s">
         <v>40</v>
@@ -1457,7 +1457,7 @@
         <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I22" t="s">
         <v>41</v>
@@ -1483,7 +1483,7 @@
         <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I23" t="s">
         <v>42</v>
@@ -1509,7 +1509,7 @@
         <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I24" t="s">
         <v>43</v>
@@ -1535,7 +1535,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I25" t="s">
         <v>44</v>
@@ -1561,7 +1561,7 @@
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I26" t="s">
         <v>92</v>
@@ -1587,7 +1587,7 @@
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I27" t="s">
         <v>83</v>
@@ -1613,7 +1613,7 @@
         <v>58</v>
       </c>
       <c r="H28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I28" t="s">
         <v>45</v>
@@ -1640,7 +1640,7 @@
         <v>51</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>93</v>
@@ -1666,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I30" t="s">
         <v>46</v>
@@ -1692,7 +1692,7 @@
         <v>51</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I31" t="s">
         <v>94</v>
@@ -1718,7 +1718,7 @@
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I32" t="s">
         <v>88</v>
@@ -1744,7 +1744,7 @@
         <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I33" t="s">
         <v>95</v>
@@ -1770,7 +1770,7 @@
         <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I34" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
build overview table from postgres and PSCIS (when possible).  Backed up old Parsnip_report.Rmd file in drafts on personal drive
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD52AF2-4E16-4F3F-BAF6-5ECFBB24F8B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D453F91-C7C0-4566-AEDB-4826C0506042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
   <sheets>
     <sheet name="priorities" sheetId="1" r:id="rId1"/>
-    <sheet name="bt_critical" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$G$1:$G$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$H$1:$H$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
     <author>tc={62D18BF9-B4D1-4E85-A958-96B85D2D3486}</author>
   </authors>
   <commentList>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -51,7 +50,7 @@
     flows into potential juv bt critical habitat</t>
       </text>
     </comment>
-    <comment ref="C21" authorId="1" shapeId="0" xr:uid="{62D18BF9-B4D1-4E85-A958-96B85D2D3486}">
+    <comment ref="D21" authorId="1" shapeId="0" xr:uid="{62D18BF9-B4D1-4E85-A958-96B85D2D3486}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
   <si>
     <t xml:space="preserve">Good habitat.  Surveyed upstream for 520 m.  Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
   </si>
@@ -243,69 +242,6 @@
     <t>Moderate</t>
   </si>
   <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>Mainstem</t>
-  </si>
-  <si>
-    <t>Juveniles</t>
-  </si>
-  <si>
-    <t>VO</t>
-  </si>
-  <si>
-    <t>Spawning</t>
-  </si>
-  <si>
-    <t>Missinka</t>
-  </si>
-  <si>
-    <t>236-614900-52600</t>
-  </si>
-  <si>
-    <t>Spawning,Juveniles</t>
-  </si>
-  <si>
-    <t>EF,VO</t>
-  </si>
-  <si>
-    <t>Wichcika</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Upper mainstem </t>
-  </si>
-  <si>
-    <t>EF</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Watershed</t>
-  </si>
-  <si>
-    <t>Section</t>
-  </si>
-  <si>
-    <t>Critical</t>
-  </si>
-  <si>
-    <t>Sampling</t>
-  </si>
-  <si>
-    <t>Information_adequacy</t>
-  </si>
-  <si>
-    <t>easting</t>
-  </si>
-  <si>
-    <t>northing</t>
-  </si>
-  <si>
-    <t>zone</t>
-  </si>
-  <si>
     <t>sort</t>
   </si>
   <si>
@@ -429,9 +365,6 @@
     <t>Young of year observed approximately 100 m downstream of crossing.  Abundant gravels throughout.</t>
   </si>
   <si>
-    <t>Small stream with low flow indicated by moss mid-channel.  Very few polls but sections of gravel present.</t>
-  </si>
-  <si>
     <t>Small stream with low flows.</t>
   </si>
   <si>
@@ -456,9 +389,6 @@
     <t>Culvert is very long, steep and continous under the CN railway and Chuchinka-Colbourne FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
   </si>
   <si>
-    <t>Multiple rock chutes up to 1 m high in surveyed area with 1.4 m falls at top end of ste.  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observed approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
   </si>
   <si>
@@ -478,6 +408,15 @@
   </si>
   <si>
     <t>Beaver influenced wetland/stream complex below crossing.  Deep glide habitat throughout (90 cm deep at time of survey).</t>
+  </si>
+  <si>
+    <t>model_crossing_id</t>
+  </si>
+  <si>
+    <t>Small stream with low flow indicated by moss mid-channel.  Very few pools but sections of gravel present.</t>
+  </si>
+  <si>
+    <t>Multiple drops and rock chutes beginning 350 m upstream of culvert with 1.4 m falls at top end of site (650 m upstream of culvert).  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observed approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
   </si>
 </sst>
 </file>
@@ -859,10 +798,10 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G10" dT="2020-04-18T20:31:59.51" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
+  <threadedComment ref="H10" dT="2020-04-18T20:31:59.51" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{4D391422-F0CF-470F-88EC-6652FF5BB05D}">
     <text>flows into potential juv bt critical habitat</text>
   </threadedComment>
-  <threadedComment ref="C21" dT="2020-03-02T16:45:41.92" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{62D18BF9-B4D1-4E85-A958-96B85D2D3486}">
+  <threadedComment ref="D21" dT="2020-03-02T16:45:41.92" personId="{EDC48F15-7FAD-4CBF-96A2-956D0112F629}" id="{62D18BF9-B4D1-4E85-A958-96B85D2D3486}">
     <text>estimate.  do I have track from JJ?</text>
   </threadedComment>
 </ThreadedComments>
@@ -870,574 +809,578 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="41.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="88.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="5" max="6" width="41.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="88.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>49</v>
       </c>
       <c r="C1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>700</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="F2" t="s">
-        <v>91</v>
-      </c>
       <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
         <v>50</v>
       </c>
-      <c r="H2" t="s">
-        <v>99</v>
-      </c>
       <c r="I2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>650</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
       </c>
-      <c r="F3" t="s">
-        <v>91</v>
-      </c>
       <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
         <v>50</v>
       </c>
-      <c r="H3" t="s">
-        <v>101</v>
-      </c>
       <c r="I3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="J3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>565</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="F4" t="s">
-        <v>91</v>
-      </c>
       <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
         <v>50</v>
       </c>
-      <c r="H4" t="s">
-        <v>102</v>
-      </c>
       <c r="I4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>400</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="F5" t="s">
-        <v>91</v>
-      </c>
       <c r="G5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" t="s">
         <v>50</v>
       </c>
-      <c r="H5" t="s">
-        <v>104</v>
-      </c>
       <c r="I5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>520</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" t="s">
         <v>51</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>360</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
       <c r="G7" t="s">
         <v>51</v>
       </c>
       <c r="H7" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="I7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>350</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>50</v>
       </c>
       <c r="G8" t="s">
         <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>106</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>120</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>50</v>
       </c>
       <c r="G9" t="s">
         <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="J9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>520</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>52</v>
       </c>
-      <c r="F10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="I10" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>920</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>52</v>
       </c>
-      <c r="F11" t="s">
-        <v>91</v>
-      </c>
       <c r="G11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
         <v>58</v>
       </c>
-      <c r="H11" t="s">
-        <v>111</v>
-      </c>
       <c r="I11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="J11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>650</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>52</v>
       </c>
-      <c r="F12" t="s">
-        <v>91</v>
-      </c>
       <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
         <v>58</v>
       </c>
-      <c r="H12" t="s">
-        <v>130</v>
-      </c>
       <c r="I12" t="s">
+        <v>117</v>
+      </c>
+      <c r="J12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>260</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>52</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" t="s">
         <v>91</v>
       </c>
-      <c r="G13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" t="s">
-        <v>112</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>350</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
-        <v>89</v>
-      </c>
       <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G14" t="s">
         <v>51</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="I14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>325</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>54</v>
       </c>
-      <c r="F15" t="s">
-        <v>51</v>
-      </c>
       <c r="G15" t="s">
         <v>51</v>
       </c>
       <c r="H15" t="s">
-        <v>137</v>
+        <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="J15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>50</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>53</v>
-      </c>
-      <c r="F16" t="s">
-        <v>50</v>
       </c>
       <c r="G16" t="s">
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="I16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>75</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>53</v>
-      </c>
-      <c r="F17" t="s">
-        <v>50</v>
       </c>
       <c r="G17" t="s">
         <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="I17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>350</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="I18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>600</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>55</v>
       </c>
-      <c r="F19" t="s">
-        <v>51</v>
-      </c>
       <c r="G19" t="s">
         <v>51</v>
       </c>
       <c r="H19" t="s">
-        <v>132</v>
+        <v>51</v>
       </c>
       <c r="I19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>755</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>54</v>
       </c>
-      <c r="F20" t="s">
-        <v>51</v>
-      </c>
       <c r="G20" t="s">
         <v>51</v>
       </c>
       <c r="H20" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="I20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="J20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>190</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>54</v>
       </c>
-      <c r="F21" t="s">
-        <v>51</v>
-      </c>
       <c r="G21" t="s">
         <v>51</v>
       </c>
       <c r="H21" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="I21" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1445,25 +1388,28 @@
         <v>33</v>
       </c>
       <c r="C22">
+        <v>16603266</v>
+      </c>
+      <c r="D22">
         <v>310</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>55</v>
       </c>
-      <c r="F22" t="s">
-        <v>51</v>
-      </c>
       <c r="G22" t="s">
         <v>51</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="I22" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1471,486 +1417,319 @@
         <v>34</v>
       </c>
       <c r="C23">
+        <v>16603266</v>
+      </c>
+      <c r="D23">
         <v>425</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>55</v>
       </c>
-      <c r="F23" t="s">
-        <v>51</v>
-      </c>
       <c r="G23" t="s">
         <v>51</v>
       </c>
       <c r="H23" t="s">
-        <v>135</v>
+        <v>51</v>
       </c>
       <c r="I23" t="s">
+        <v>112</v>
+      </c>
+      <c r="J23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>800</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>54</v>
       </c>
-      <c r="F24" t="s">
-        <v>51</v>
-      </c>
       <c r="G24" t="s">
         <v>51</v>
       </c>
       <c r="H24" t="s">
-        <v>118</v>
+        <v>51</v>
       </c>
       <c r="I24" t="s">
+        <v>97</v>
+      </c>
+      <c r="J24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>240</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>54</v>
       </c>
-      <c r="F25" t="s">
-        <v>51</v>
-      </c>
       <c r="G25" t="s">
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>127</v>
+        <v>51</v>
       </c>
       <c r="I25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26">
+        <v>60</v>
+      </c>
+      <c r="D26">
         <v>680</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>54</v>
       </c>
-      <c r="F26" t="s">
-        <v>51</v>
-      </c>
       <c r="G26" t="s">
         <v>51</v>
       </c>
       <c r="H26" t="s">
-        <v>126</v>
+        <v>51</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="J26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27">
+        <v>61</v>
+      </c>
+      <c r="D27">
         <v>220</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>54</v>
       </c>
-      <c r="F27" t="s">
-        <v>51</v>
-      </c>
       <c r="G27" t="s">
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="I27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>550</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>54</v>
       </c>
-      <c r="F28" t="s">
-        <v>91</v>
-      </c>
       <c r="G28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" t="s">
         <v>58</v>
       </c>
-      <c r="H28" t="s">
-        <v>129</v>
-      </c>
       <c r="I28" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2">
         <v>530</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="4" t="s">
+      <c r="F29" s="2"/>
+      <c r="G29" t="s">
         <v>51</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>27</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>600</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>53</v>
       </c>
-      <c r="F30" t="s">
-        <v>51</v>
-      </c>
       <c r="G30" t="s">
         <v>51</v>
       </c>
       <c r="H30" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
       <c r="I30" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>28</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>400</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>53</v>
       </c>
-      <c r="F31" t="s">
-        <v>51</v>
-      </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" t="s">
         <v>51</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="I31" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="J31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>525</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>53</v>
       </c>
-      <c r="F32" t="s">
-        <v>51</v>
-      </c>
       <c r="G32" t="s">
         <v>51</v>
       </c>
       <c r="H32" t="s">
-        <v>120</v>
+        <v>51</v>
       </c>
       <c r="I32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="J32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>30</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>295</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>54</v>
-      </c>
-      <c r="F33" t="s">
-        <v>91</v>
       </c>
       <c r="G33" t="s">
         <v>50</v>
       </c>
       <c r="H33" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="J33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>31</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>215</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>54</v>
-      </c>
-      <c r="F34" t="s">
-        <v>91</v>
       </c>
       <c r="G34" t="s">
         <v>50</v>
       </c>
       <c r="H34" t="s">
-        <v>122</v>
+        <v>50</v>
       </c>
       <c r="I34" t="s">
+        <v>100</v>
+      </c>
+      <c r="J34" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C38">
-        <f>SUM(C2:C35)</f>
-        <v>14690</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="G1:G38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
+  <autoFilter ref="H1:H38" xr:uid="{8E415BEC-1355-41FC-886A-514C5C27A9AA}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9D27EBA-D289-4F52-B229-A21218E79CD2}">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>564904</v>
-      </c>
-      <c r="I2">
-        <v>6074167</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3">
-        <v>560080</v>
-      </c>
-      <c r="I3">
-        <v>6070504</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>582085</v>
-      </c>
-      <c r="I4">
-        <v>6051256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>559123</v>
-      </c>
-      <c r="I5">
-        <v>6039919</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
work on crossing appendices template.  rebuild functions to make objects that are multi-referenced.
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D453F91-C7C0-4566-AEDB-4826C0506042}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524352E6-6583-4994-847D-7D148BFA6A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
@@ -386,9 +386,6 @@
     <t>Abundant undercut banks, overhanging vegetation, large woody debris and gravels.  Historic beaver dam 700 m upstream.  Railway culvert (modelled crossing 16603287) is  200 m upstream and is barrier (90 m long, unembedded and 3%).</t>
   </si>
   <si>
-    <t>Culvert is very long, steep and continous under the CN railway and Chuchinka-Colbourne FSR (PSCIS 125353) and empties directly into margins of Parsnip River.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Classified as fisheries sensitive watershed under FRPA due to downstream Bull Trout and Arctic Grayling (Beaudry 2013, FSW-TAG f-7-020). Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>Multiple drops and rock chutes beginning 350 m upstream of culvert with 1.4 m falls at top end of site (650 m upstream of culvert).  Deep pools suitable for overwintering and rearing.  Rainbow trout (120 mm) observed approximately 60 m upstream of culvert.  Some gravels present suitable for spawning present.</t>
+  </si>
+  <si>
+    <t>The culvert is very long, steep and continous under the CN railway and Chuchinka-Colbourne FSR (PSCIS crossing 125353) and empties directly into margins of Parsnip River.  Stream drains Goose Lake. Numerous fish observed upstream.  Small woody debris, overhanging vegetation and undercut banks abundant.  Some  gravels present suitable for spawning.  Minnowtrapping conducted upsteam and downstream. Rainbow trout captured upstream and burbot and rainbow trout captured downstream.</t>
   </si>
 </sst>
 </file>
@@ -811,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +833,7 @@
         <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
         <v>24</v>
@@ -981,7 +981,7 @@
         <v>51</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
         <v>0</v>
@@ -1137,7 +1137,7 @@
         <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J12" t="s">
         <v>3</v>
@@ -1218,7 +1218,7 @@
         <v>51</v>
       </c>
       <c r="I15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J15" t="s">
         <v>64</v>
@@ -1244,7 +1244,7 @@
         <v>50</v>
       </c>
       <c r="I16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J16" t="s">
         <v>5</v>
@@ -1322,7 +1322,7 @@
         <v>51</v>
       </c>
       <c r="I19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J19" t="s">
         <v>66</v>
@@ -1432,7 +1432,7 @@
         <v>51</v>
       </c>
       <c r="I23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J23" t="s">
         <v>42</v>
@@ -1562,7 +1562,7 @@
         <v>58</v>
       </c>
       <c r="I28" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="J28" t="s">
         <v>45</v>
@@ -1590,7 +1590,7 @@
         <v>51</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>72</v>
@@ -1642,7 +1642,7 @@
         <v>51</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J31" t="s">
         <v>73</v>
@@ -1694,7 +1694,7 @@
         <v>50</v>
       </c>
       <c r="I33" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J33" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
remove extra sheet from priorities
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-010_FWCP_Parsnip\scripts\main\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE85F1C-20F4-489F-B324-BF07683C4D8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE7504D-6592-4BA0-8F23-4EA6EDD0D647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8240AFED-DFEA-4E94-B412-33551FE32823}"/>
   </bookViews>
   <sheets>
     <sheet name="priorities" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">priorities!$H$1:$H$38</definedName>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
   <si>
     <t xml:space="preserve">Good habitat.  Surveyed upstream for 520 m.  Some deep pools for overwintering and rearing.  Large woody debris and undercut banks throughout. Sections of gravel suitable for spawning.  Good flow.  </t>
   </si>
@@ -418,42 +417,6 @@
   </si>
   <si>
     <t>The culvert is very long, steep and continous under the CN railway and Chuchinka-Colbourne FSR (PSCIS crossing 125353) and empties directly into margins of Parsnip River.  Stream drains Goose Lake. Numerous fish observed upstream.  Small woody debris, overhanging vegetation and undercut banks abundant.  Some  gravels present suitable for spawning.  Minnowtrapping conducted upsteam and downstream. Rainbow trout captured upstream and burbot and rainbow trout captured downstream.</t>
-  </si>
-  <si>
-    <t>barrier</t>
-  </si>
-  <si>
-    <t>stream_barred_perc</t>
-  </si>
-  <si>
-    <t>limiting_to_upstream_barrier</t>
-  </si>
-  <si>
-    <t>fish_species</t>
-  </si>
-  <si>
-    <t>habitat_value</t>
-  </si>
-  <si>
-    <t>length_of_new_habitat</t>
-  </si>
-  <si>
-    <t>fish_species_score</t>
-  </si>
-  <si>
-    <t>habitat_value_score</t>
-  </si>
-  <si>
-    <t>barrier_score</t>
-  </si>
-  <si>
-    <t>length_of_new_habitat_score</t>
-  </si>
-  <si>
-    <t>stream_barred_perc_score</t>
-  </si>
-  <si>
-    <t>limiting_to_upstream_barrier_score</t>
   </si>
 </sst>
 </file>
@@ -509,13 +472,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -849,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828D4784-30D9-4AED-B616-3E5AC19D34FC}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,236 +1732,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9201A1C-8BB4-4FFE-98FF-E543BD1AFEC2}">
-  <dimension ref="A1:M34"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I1" t="s">
-        <v>127</v>
-      </c>
-      <c r="J1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" t="s">
-        <v>119</v>
-      </c>
-      <c r="L1" t="s">
-        <v>120</v>
-      </c>
-      <c r="M1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>